<commit_message>
added offerte en use case
</commit_message>
<xml_diff>
--- a/documenten/kerntaak_1/1.1/offerte/offerte.xlsx
+++ b/documenten/kerntaak_1/1.1/offerte/offerte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\did-you-had-a-good-day\documenten\kerntaak_1\1.1\offerte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D360598-1DB0-4055-82F8-116AF51DCE5B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52649265-8164-4CF9-BA29-53A6B2108A5D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{4DFF705B-AE8A-479A-9771-2604BBCB6A80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Wilhelminasingel 33</t>
   </si>
@@ -72,9 +72,6 @@
     <t>ontwikkeling van de applicatie (in uren)</t>
   </si>
   <si>
-    <t xml:space="preserve">live zetten van de applicatie </t>
-  </si>
-  <si>
     <t>subtotaal</t>
   </si>
   <si>
@@ -85,12 +82,30 @@
   </si>
   <si>
     <t>Totaal</t>
+  </si>
+  <si>
+    <t>Terheijdenseweg 350</t>
+  </si>
+  <si>
+    <t>4826 AA Breda</t>
+  </si>
+  <si>
+    <t>mail: kf100831@edu.rocwb.nl</t>
+  </si>
+  <si>
+    <t>raduis college</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mail: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,12 +135,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -442,126 +461,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542DED0B-3B70-458D-8CC2-91B7AC606FA1}">
-  <dimension ref="A4:E26"/>
+  <dimension ref="A4:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B14" s="2">
         <v>43187</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="C16">
+      <c r="C19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D19" s="4">
+        <v>100</v>
+      </c>
+      <c r="E19" s="4">
+        <f>C19*D19</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="C20" s="1">
         <v>216</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D20" s="4">
+        <v>55</v>
+      </c>
+      <c r="E20" s="4">
+        <f>C20*D20</f>
+        <v>11880</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="E25" s="4">
+        <f>E19+E20+E21</f>
+        <v>11980</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="E27" s="4">
+        <f>E25/100*21</f>
+        <v>2515.7999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>19</v>
+      <c r="E29" s="4">
+        <f>E25+E26+E27</f>
+        <v>14495.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes documenten herkansing kt1
</commit_message>
<xml_diff>
--- a/documenten/kerntaak_1/1.1/offerte/offerte.xlsx
+++ b/documenten/kerntaak_1/1.1/offerte/offerte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\did-you-had-a-good-day\documenten\kerntaak_1\1.1\offerte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1366FDDF-A548-41F3-8766-9912D6582EB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328F6B54-9037-49B0-AE98-FA39049AAB5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,14 +582,14 @@
         <v>11</v>
       </c>
       <c r="C21" s="1">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="D21" s="4">
         <v>55</v>
       </c>
       <c r="E21" s="4">
         <f>C21*D21</f>
-        <v>11880</v>
+        <v>9075</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -601,8 +601,8 @@
         <v>10</v>
       </c>
       <c r="E26" s="4">
-        <f>E20+E21+E22</f>
-        <v>11980</v>
+        <f>SUM(E20:E25)</f>
+        <v>9175</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
       </c>
       <c r="E28" s="4">
         <f>E26/100*21</f>
-        <v>2515.7999999999997</v>
+        <v>1926.75</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -629,7 +629,7 @@
       </c>
       <c r="E30" s="4">
         <f>E26+E27+E28</f>
-        <v>14495.8</v>
+        <v>11101.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>